<commit_message>
ksu002 b export update
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
@@ -13,7 +13,6 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">ksu002B!$4:$9</definedName>
@@ -43,12 +42,12 @@
     <definedName function="false" hidden="false" name="LBlue1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="LBlue2" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="LBlue3" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="OPT_NO" vbProcedure="false">[5]!OPT_NO</definedName>
-    <definedName function="false" hidden="false" name="OPT_YES" vbProcedure="false">[5]!OPT_YES</definedName>
+    <definedName function="false" hidden="false" name="OPT_NO" vbProcedure="false">[5]!opt_no</definedName>
+    <definedName function="false" hidden="false" name="OPT_YES" vbProcedure="false">[5]!opt_yes</definedName>
     <definedName function="false" hidden="false" name="PG単価" vbProcedure="false">[6]明細合計!#REF!</definedName>
     <definedName function="false" hidden="false" name="PG田中" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="PrintDaicho" vbProcedure="false">[7]!PrintDaicho</definedName>
-    <definedName function="false" hidden="false" name="QuitDaicho" vbProcedure="false">[7]!QuitDaicho</definedName>
+    <definedName function="false" hidden="false" name="PrintDaicho" vbProcedure="false">[7]!printdaicho</definedName>
+    <definedName function="false" hidden="false" name="QuitDaicho" vbProcedure="false">[7]!quitdaicho</definedName>
     <definedName function="false" hidden="false" name="REMARK" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="SE単価" vbProcedure="false">[6]明細合計!#REF!</definedName>
     <definedName function="false" hidden="false" name="SS単価" vbProcedure="false">#REF!</definedName>
@@ -86,7 +85,7 @@
     <definedName function="false" hidden="false" name="サホ1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="サＨ" vbProcedure="false">[8]１．社内ﾈｯﾄﾜｰｸﾊｰﾄﾞｳｪｱ!#REF!</definedName>
     <definedName function="false" hidden="false" name="ツール別見積工数" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" name="テーブル項目" vbProcedure="false">[9]項目定義書!$A$3:$E$364</definedName>
+    <definedName function="false" hidden="false" name="テーブル項目" vbProcedure="false">[9]項目定義書!$a$3:#REF!</definedName>
     <definedName function="false" hidden="false" name="ハサホ" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="ハホ" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="ハ１" vbProcedure="false">#REF!</definedName>
@@ -117,7 +116,7 @@
     <definedName function="false" hidden="false" name="日帰り単金" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="概要_基準日設定" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="標準価格" vbProcedure="false">'[2]見積明細(ハードのみ）'!$C$5:$H$34</definedName>
-    <definedName function="false" hidden="false" name="機種SORT" vbProcedure="false">[11]!機種SORT</definedName>
+    <definedName function="false" hidden="false" name="機種SORT" vbProcedure="false">[11]!機種sort</definedName>
     <definedName function="false" hidden="false" name="機能別原価" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" name="直扱単価" vbProcedure="false">'[2]見積明細(ハードのみ）'!$V$5:$V$34</definedName>
     <definedName function="false" hidden="false" name="社共単価" vbProcedure="false">'[2]見積明細(ハードのみ）'!$T$5:$T$34</definedName>
@@ -154,12 +153,12 @@
     <definedName function="false" hidden="false" localSheetId="0" name="def" vbProcedure="false">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="item1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="kkkk" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="OPT_NO" vbProcedure="false">[5]!OPT_NO</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="OPT_YES" vbProcedure="false">[5]!OPT_YES</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="OPT_NO" vbProcedure="false">[5]!opt_no</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="OPT_YES" vbProcedure="false">[5]!opt_yes</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="PG単価" vbProcedure="false">[6]明細合計!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="PG田中" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="PrintDaicho" vbProcedure="false">[7]!PrintDaicho</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="QuitDaicho" vbProcedure="false">[7]!QuitDaicho</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="PrintDaicho" vbProcedure="false">[7]!printdaicho</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="QuitDaicho" vbProcedure="false">[7]!quitdaicho</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="SE単価" vbProcedure="false">[6]明細合計!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="SS単価" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="STEP概算" vbProcedure="false">#REF!</definedName>
@@ -243,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t xml:space="preserve">A1_1</t>
   </si>
@@ -302,16 +301,58 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
+    <t xml:space="preserve"> &amp;=item.coln1C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;=coln1C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln2C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;=coln2C22 </t>
+  </si>
+  <si>
     <t xml:space="preserve">C2_1</t>
   </si>
   <si>
     <t xml:space="preserve">C2_2</t>
   </si>
   <si>
+    <t xml:space="preserve"> &amp;=item.coln1C231</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln1C232</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln2C231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;=item.coln2C232</t>
+  </si>
+  <si>
     <t xml:space="preserve">C2_3_1</t>
   </si>
   <si>
     <t xml:space="preserve">C2_3_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln1C233</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln1C235</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln1C234</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln2C233</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln2C235</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;=item.coln2C234</t>
   </si>
   <si>
     <t xml:space="preserve">C2_3_3</t>
@@ -379,6 +420,7 @@
       <color rgb="FF000000"/>
       <name val="ＭＳ ゴシック"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -562,7 +604,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -684,19 +726,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="仕切価格"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="項目定義書"/>
     </sheetNames>
     <sheetDataSet>
@@ -714,11 +743,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ7" activeCellId="0" sqref="AJ7"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC16" activeCellId="0" sqref="AC16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.15625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="3.1640625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.86"/>
@@ -2174,59 +2203,59 @@
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L12" s="23"/>
       <c r="M12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O12" s="22"/>
       <c r="P12" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q12" s="23"/>
       <c r="R12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="T12" s="22"/>
       <c r="U12" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="V12" s="23"/>
       <c r="W12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Y12" s="22"/>
       <c r="Z12" s="23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AA12" s="23"/>
       <c r="AB12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AD12" s="22"/>
       <c r="AE12" s="23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AF12" s="23"/>
       <c r="AG12" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AI12" s="22"/>
       <c r="AJ12" s="23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="AK12" s="23"/>
       <c r="AL12" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="AN12" s="22"/>
     </row>
@@ -2243,75 +2272,75 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="21" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
       <c r="D14" s="25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="J14" s="25"/>
       <c r="K14" s="23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="L14" s="23"/>
       <c r="M14" s="23"/>
       <c r="N14" s="25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="O14" s="25"/>
       <c r="P14" s="23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="Q14" s="23"/>
       <c r="R14" s="23"/>
       <c r="S14" s="25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="T14" s="25"/>
       <c r="U14" s="23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="V14" s="23"/>
       <c r="W14" s="23"/>
       <c r="X14" s="25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="Y14" s="25"/>
       <c r="Z14" s="23" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="AA14" s="23"/>
       <c r="AB14" s="23"/>
       <c r="AC14" s="25" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="AD14" s="25"/>
       <c r="AE14" s="23" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="AF14" s="23"/>
       <c r="AG14" s="23"/>
       <c r="AH14" s="25" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AI14" s="25"/>
       <c r="AJ14" s="23" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="AK14" s="23"/>
       <c r="AL14" s="23"/>
       <c r="AM14" s="25" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AN14" s="25"/>
     </row>
@@ -2328,91 +2357,91 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G16" s="27"/>
       <c r="H16" s="27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="I16" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="L16" s="27"/>
       <c r="M16" s="27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="N16" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="O16" s="28"/>
       <c r="P16" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="27"/>
       <c r="R16" s="27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="S16" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="T16" s="28"/>
       <c r="U16" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="V16" s="27"/>
       <c r="W16" s="27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="X16" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="Y16" s="28"/>
       <c r="Z16" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="AA16" s="27"/>
       <c r="AB16" s="27" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="AC16" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="AD16" s="28"/>
       <c r="AE16" s="27" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="AF16" s="27"/>
       <c r="AG16" s="27" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="AH16" s="28" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="AI16" s="28"/>
       <c r="AJ16" s="27" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="AK16" s="27"/>
       <c r="AL16" s="27" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="AM16" s="28" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="AN16" s="28"/>
     </row>
@@ -2478,7 +2507,7 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"源ノ角ゴシック Normal,Bold"&amp;16日別勤務表&amp;R&amp;"源ノ角ゴシック Normal,Regular"&amp;D　&amp;T　
 page&amp;P</oddHeader>
-    <oddFooter>&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過 </oddFooter>
+    <oddFooter>&amp;L備考　未マ：マスタ未登録、漏れ：打刻漏れ、打順：打刻順序不正、遅：遅刻、早：早退、休打：休日打刻、二重：二重打刻、反映：承認反映、手：手入力、未計：未計算、申超：事前申請超過</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#56847 has been resolved
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
@@ -15,28 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
-  <si>
-    <t>日</t>
-  </si>
-  <si>
-    <t>月</t>
-  </si>
-  <si>
-    <t>火</t>
-  </si>
-  <si>
-    <t>水</t>
-  </si>
-  <si>
-    <t>木</t>
-  </si>
-  <si>
-    <t>金</t>
-  </si>
-  <si>
-    <t>土</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>週合計</t>
   </si>
@@ -46,10 +25,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -64,30 +43,6 @@
       <color theme="1"/>
       <name val="MS ゴシック"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -106,14 +61,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,8 +82,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,15 +107,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,23 +129,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,27 +166,28 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -225,18 +204,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -249,37 +306,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +336,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,103 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,6 +516,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -566,35 +580,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,19 +607,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,15 +617,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -656,134 +635,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -848,12 +827,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -1181,7 +1154,7 @@
   <dimension ref="A3:AN33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4:AN4"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.13888888888889" defaultRowHeight="14.1" customHeight="1"/>
@@ -1190,51 +1163,37 @@
   </cols>
   <sheetData>
     <row r="3" customHeight="1" spans="1:40">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="U3" s="2"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="4"/>
-      <c r="Z3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="Z3" s="2"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="4"/>
-      <c r="AE3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AE3" s="2"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
@@ -1282,10 +1241,10 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="7"/>
       <c r="AJ4" s="21"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="23"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="16"/>
+      <c r="AM4" s="16"/>
+      <c r="AN4" s="17"/>
     </row>
     <row r="5" customHeight="1" spans="1:40">
       <c r="A5" s="8"/>
@@ -1378,9 +1337,9 @@
       <c r="AH8" s="11"/>
       <c r="AI8" s="12"/>
       <c r="AJ8" s="8"/>
-      <c r="AK8" s="24"/>
-      <c r="AL8" s="24"/>
-      <c r="AM8" s="24"/>
+      <c r="AK8" s="22"/>
+      <c r="AL8" s="22"/>
+      <c r="AM8" s="22"/>
       <c r="AN8" s="9"/>
     </row>
     <row r="9" customHeight="1" spans="1:40">
@@ -1513,9 +1472,9 @@
       <c r="AH13" s="11"/>
       <c r="AI13" s="12"/>
       <c r="AJ13" s="8"/>
-      <c r="AK13" s="24"/>
-      <c r="AL13" s="24"/>
-      <c r="AM13" s="24"/>
+      <c r="AK13" s="22"/>
+      <c r="AL13" s="22"/>
+      <c r="AM13" s="22"/>
       <c r="AN13" s="9"/>
     </row>
     <row r="14" customHeight="1" spans="1:40">
@@ -1648,9 +1607,9 @@
       <c r="AH18" s="11"/>
       <c r="AI18" s="12"/>
       <c r="AJ18" s="8"/>
-      <c r="AK18" s="24"/>
-      <c r="AL18" s="24"/>
-      <c r="AM18" s="24"/>
+      <c r="AK18" s="22"/>
+      <c r="AL18" s="22"/>
+      <c r="AM18" s="22"/>
       <c r="AN18" s="9"/>
     </row>
     <row r="19" customHeight="1" spans="1:40">
@@ -1783,9 +1742,9 @@
       <c r="AH23" s="11"/>
       <c r="AI23" s="12"/>
       <c r="AJ23" s="8"/>
-      <c r="AK23" s="24"/>
-      <c r="AL23" s="24"/>
-      <c r="AM23" s="24"/>
+      <c r="AK23" s="22"/>
+      <c r="AL23" s="22"/>
+      <c r="AM23" s="22"/>
       <c r="AN23" s="9"/>
     </row>
     <row r="24" customHeight="1" spans="1:40">
@@ -1918,9 +1877,9 @@
       <c r="AH28" s="11"/>
       <c r="AI28" s="12"/>
       <c r="AJ28" s="8"/>
-      <c r="AK28" s="24"/>
-      <c r="AL28" s="24"/>
-      <c r="AM28" s="24"/>
+      <c r="AK28" s="22"/>
+      <c r="AL28" s="22"/>
+      <c r="AM28" s="22"/>
       <c r="AN28" s="9"/>
     </row>
     <row r="29" customHeight="1" spans="1:40">
@@ -2082,7 +2041,7 @@
   <dimension ref="A3:AN33"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM5" sqref="AM5:AN5"/>
+      <selection activeCell="AE3" sqref="AE3:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.13888888888889" defaultRowHeight="14.1" customHeight="1"/>
@@ -2091,57 +2050,43 @@
   </cols>
   <sheetData>
     <row r="3" customHeight="1" spans="1:40">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4"/>
-      <c r="U3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="U3" s="2"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="4"/>
-      <c r="Z3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="Z3" s="2"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
       <c r="AD3" s="4"/>
-      <c r="AE3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="AE3" s="2"/>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="4"/>
       <c r="AJ3" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="3"/>
       <c r="AL3" s="3"/>

</xml_diff>

<commit_message>
ksu002b: focus row first when open
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
@@ -9,16 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22365" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="テンプレート  " sheetId="2" r:id="rId1"/>
     <sheet name="テンプレート   " sheetId="3" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'テンプレート  '!$A$1:$AN$33</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'テンプレート   '!$A$1:$AN$33</definedName>
-  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -254,6 +250,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -262,21 +273,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="14.1" customHeight="1"/>
   <cols>
@@ -1431,16 +1427,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="U3:Y3"/>
     <mergeCell ref="Z3:AD3"/>
     <mergeCell ref="AE3:AI3"/>
     <mergeCell ref="AJ3:AN3"/>
     <mergeCell ref="AJ4:AN4"/>
     <mergeCell ref="S1:V2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="U3:Y3"/>
   </mergeCells>
   <pageMargins left="0.389583333333333" right="0.389583333333333" top="1" bottom="0.58958333333333302" header="0.30972222222222201" footer="0.30972222222222201"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1451,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="14.1" customHeight="1"/>
   <cols>
@@ -1506,13 +1502,13 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="13"/>
-      <c r="AJ3" s="20" t="s">
+      <c r="AJ3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="22"/>
+      <c r="AK3" s="26"/>
+      <c r="AL3" s="26"/>
+      <c r="AM3" s="26"/>
+      <c r="AN3" s="27"/>
     </row>
     <row r="4" spans="1:40" ht="14.1" customHeight="1">
       <c r="A4" s="2"/>
@@ -1550,11 +1546,11 @@
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
       <c r="AI4" s="4"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="25"/>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="24"/>
     </row>
     <row r="5" spans="1:40" ht="14.1" customHeight="1">
       <c r="A5" s="5"/>
@@ -1571,9 +1567,9 @@
       <c r="AD5" s="6"/>
       <c r="AE5" s="5"/>
       <c r="AI5" s="6"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="27"/>
-      <c r="AL5" s="27"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
       <c r="AM5" s="18"/>
       <c r="AN5" s="19"/>
     </row>
@@ -1592,9 +1588,9 @@
       <c r="AD6" s="6"/>
       <c r="AE6" s="5"/>
       <c r="AI6" s="6"/>
-      <c r="AJ6" s="26"/>
-      <c r="AK6" s="27"/>
-      <c r="AL6" s="27"/>
+      <c r="AJ6" s="20"/>
+      <c r="AK6" s="21"/>
+      <c r="AL6" s="21"/>
       <c r="AM6" s="18"/>
       <c r="AN6" s="19"/>
     </row>
@@ -1613,9 +1609,9 @@
       <c r="AD7" s="6"/>
       <c r="AE7" s="5"/>
       <c r="AI7" s="6"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="27"/>
-      <c r="AL7" s="27"/>
+      <c r="AJ7" s="20"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="21"/>
       <c r="AM7" s="18"/>
       <c r="AN7" s="19"/>
     </row>
@@ -1697,11 +1693,11 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="4"/>
-      <c r="AJ9" s="23"/>
-      <c r="AK9" s="24"/>
-      <c r="AL9" s="24"/>
-      <c r="AM9" s="24"/>
-      <c r="AN9" s="25"/>
+      <c r="AJ9" s="22"/>
+      <c r="AK9" s="23"/>
+      <c r="AL9" s="23"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="24"/>
     </row>
     <row r="10" spans="1:40" ht="14.1" customHeight="1">
       <c r="A10" s="5"/>
@@ -1718,9 +1714,9 @@
       <c r="AD10" s="6"/>
       <c r="AE10" s="5"/>
       <c r="AI10" s="6"/>
-      <c r="AJ10" s="26"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="27"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="21"/>
+      <c r="AL10" s="21"/>
       <c r="AM10" s="18"/>
       <c r="AN10" s="19"/>
     </row>
@@ -1739,9 +1735,9 @@
       <c r="AD11" s="6"/>
       <c r="AE11" s="5"/>
       <c r="AI11" s="6"/>
-      <c r="AJ11" s="26"/>
-      <c r="AK11" s="27"/>
-      <c r="AL11" s="27"/>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="21"/>
+      <c r="AL11" s="21"/>
       <c r="AM11" s="18"/>
       <c r="AN11" s="19"/>
     </row>
@@ -1760,9 +1756,9 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="5"/>
       <c r="AI12" s="6"/>
-      <c r="AJ12" s="26"/>
-      <c r="AK12" s="27"/>
-      <c r="AL12" s="27"/>
+      <c r="AJ12" s="20"/>
+      <c r="AK12" s="21"/>
+      <c r="AL12" s="21"/>
       <c r="AM12" s="18"/>
       <c r="AN12" s="19"/>
     </row>
@@ -1844,11 +1840,11 @@
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="4"/>
-      <c r="AJ14" s="23"/>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="24"/>
-      <c r="AM14" s="24"/>
-      <c r="AN14" s="25"/>
+      <c r="AJ14" s="22"/>
+      <c r="AK14" s="23"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="24"/>
     </row>
     <row r="15" spans="1:40" ht="14.1" customHeight="1">
       <c r="A15" s="5"/>
@@ -1865,9 +1861,9 @@
       <c r="AD15" s="6"/>
       <c r="AE15" s="5"/>
       <c r="AI15" s="6"/>
-      <c r="AJ15" s="26"/>
-      <c r="AK15" s="27"/>
-      <c r="AL15" s="27"/>
+      <c r="AJ15" s="20"/>
+      <c r="AK15" s="21"/>
+      <c r="AL15" s="21"/>
       <c r="AM15" s="18"/>
       <c r="AN15" s="19"/>
     </row>
@@ -1886,9 +1882,9 @@
       <c r="AD16" s="6"/>
       <c r="AE16" s="5"/>
       <c r="AI16" s="6"/>
-      <c r="AJ16" s="26"/>
-      <c r="AK16" s="27"/>
-      <c r="AL16" s="27"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="21"/>
+      <c r="AL16" s="21"/>
       <c r="AM16" s="18"/>
       <c r="AN16" s="19"/>
     </row>
@@ -1907,9 +1903,9 @@
       <c r="AD17" s="6"/>
       <c r="AE17" s="5"/>
       <c r="AI17" s="6"/>
-      <c r="AJ17" s="26"/>
-      <c r="AK17" s="27"/>
-      <c r="AL17" s="27"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="21"/>
+      <c r="AL17" s="21"/>
       <c r="AM17" s="18"/>
       <c r="AN17" s="19"/>
     </row>
@@ -1991,11 +1987,11 @@
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="4"/>
-      <c r="AJ19" s="23"/>
-      <c r="AK19" s="24"/>
-      <c r="AL19" s="24"/>
-      <c r="AM19" s="24"/>
-      <c r="AN19" s="25"/>
+      <c r="AJ19" s="22"/>
+      <c r="AK19" s="23"/>
+      <c r="AL19" s="23"/>
+      <c r="AM19" s="23"/>
+      <c r="AN19" s="24"/>
     </row>
     <row r="20" spans="1:40" ht="14.1" customHeight="1">
       <c r="A20" s="5"/>
@@ -2012,9 +2008,9 @@
       <c r="AD20" s="6"/>
       <c r="AE20" s="5"/>
       <c r="AI20" s="6"/>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="27"/>
-      <c r="AL20" s="27"/>
+      <c r="AJ20" s="20"/>
+      <c r="AK20" s="21"/>
+      <c r="AL20" s="21"/>
       <c r="AM20" s="18"/>
       <c r="AN20" s="19"/>
     </row>
@@ -2033,9 +2029,9 @@
       <c r="AD21" s="6"/>
       <c r="AE21" s="5"/>
       <c r="AI21" s="6"/>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="27"/>
-      <c r="AL21" s="27"/>
+      <c r="AJ21" s="20"/>
+      <c r="AK21" s="21"/>
+      <c r="AL21" s="21"/>
       <c r="AM21" s="18"/>
       <c r="AN21" s="19"/>
     </row>
@@ -2054,9 +2050,9 @@
       <c r="AD22" s="6"/>
       <c r="AE22" s="5"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="26"/>
-      <c r="AK22" s="27"/>
-      <c r="AL22" s="27"/>
+      <c r="AJ22" s="20"/>
+      <c r="AK22" s="21"/>
+      <c r="AL22" s="21"/>
       <c r="AM22" s="18"/>
       <c r="AN22" s="19"/>
     </row>
@@ -2138,11 +2134,11 @@
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="4"/>
-      <c r="AJ24" s="23"/>
-      <c r="AK24" s="24"/>
-      <c r="AL24" s="24"/>
-      <c r="AM24" s="24"/>
-      <c r="AN24" s="25"/>
+      <c r="AJ24" s="22"/>
+      <c r="AK24" s="23"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="23"/>
+      <c r="AN24" s="24"/>
     </row>
     <row r="25" spans="1:40" ht="14.1" customHeight="1">
       <c r="A25" s="5"/>
@@ -2159,9 +2155,9 @@
       <c r="AD25" s="6"/>
       <c r="AE25" s="5"/>
       <c r="AI25" s="6"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="27"/>
-      <c r="AL25" s="27"/>
+      <c r="AJ25" s="20"/>
+      <c r="AK25" s="21"/>
+      <c r="AL25" s="21"/>
       <c r="AM25" s="18"/>
       <c r="AN25" s="19"/>
     </row>
@@ -2180,9 +2176,9 @@
       <c r="AD26" s="6"/>
       <c r="AE26" s="5"/>
       <c r="AI26" s="6"/>
-      <c r="AJ26" s="26"/>
-      <c r="AK26" s="27"/>
-      <c r="AL26" s="27"/>
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="21"/>
+      <c r="AL26" s="21"/>
       <c r="AM26" s="18"/>
       <c r="AN26" s="19"/>
     </row>
@@ -2201,9 +2197,9 @@
       <c r="AD27" s="6"/>
       <c r="AE27" s="5"/>
       <c r="AI27" s="6"/>
-      <c r="AJ27" s="26"/>
-      <c r="AK27" s="27"/>
-      <c r="AL27" s="27"/>
+      <c r="AJ27" s="20"/>
+      <c r="AK27" s="21"/>
+      <c r="AL27" s="21"/>
       <c r="AM27" s="18"/>
       <c r="AN27" s="19"/>
     </row>
@@ -2285,11 +2281,11 @@
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="4"/>
-      <c r="AJ29" s="23"/>
-      <c r="AK29" s="24"/>
-      <c r="AL29" s="24"/>
-      <c r="AM29" s="24"/>
-      <c r="AN29" s="25"/>
+      <c r="AJ29" s="22"/>
+      <c r="AK29" s="23"/>
+      <c r="AL29" s="23"/>
+      <c r="AM29" s="23"/>
+      <c r="AN29" s="24"/>
     </row>
     <row r="30" spans="1:40" ht="14.1" customHeight="1">
       <c r="A30" s="5"/>
@@ -2306,9 +2302,9 @@
       <c r="AD30" s="6"/>
       <c r="AE30" s="5"/>
       <c r="AI30" s="6"/>
-      <c r="AJ30" s="26"/>
-      <c r="AK30" s="27"/>
-      <c r="AL30" s="27"/>
+      <c r="AJ30" s="20"/>
+      <c r="AK30" s="21"/>
+      <c r="AL30" s="21"/>
       <c r="AM30" s="18"/>
       <c r="AN30" s="19"/>
     </row>
@@ -2327,9 +2323,9 @@
       <c r="AD31" s="6"/>
       <c r="AE31" s="5"/>
       <c r="AI31" s="6"/>
-      <c r="AJ31" s="26"/>
-      <c r="AK31" s="27"/>
-      <c r="AL31" s="27"/>
+      <c r="AJ31" s="20"/>
+      <c r="AK31" s="21"/>
+      <c r="AL31" s="21"/>
       <c r="AM31" s="18"/>
       <c r="AN31" s="19"/>
     </row>
@@ -2348,9 +2344,9 @@
       <c r="AD32" s="6"/>
       <c r="AE32" s="5"/>
       <c r="AI32" s="6"/>
-      <c r="AJ32" s="26"/>
-      <c r="AK32" s="27"/>
-      <c r="AL32" s="27"/>
+      <c r="AJ32" s="20"/>
+      <c r="AK32" s="21"/>
+      <c r="AL32" s="21"/>
       <c r="AM32" s="18"/>
       <c r="AN32" s="19"/>
     </row>
@@ -2398,6 +2394,41 @@
     </row>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="K3:O3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AJ3:AN3"/>
+    <mergeCell ref="AJ4:AN4"/>
+    <mergeCell ref="AJ5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AJ6:AL6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="AJ9:AN9"/>
+    <mergeCell ref="AJ10:AL10"/>
+    <mergeCell ref="AM10:AN10"/>
+    <mergeCell ref="AJ11:AL11"/>
+    <mergeCell ref="AM11:AN11"/>
+    <mergeCell ref="AJ12:AL12"/>
+    <mergeCell ref="AM12:AN12"/>
+    <mergeCell ref="AJ14:AN14"/>
+    <mergeCell ref="AJ15:AL15"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="AJ16:AL16"/>
+    <mergeCell ref="AM16:AN16"/>
+    <mergeCell ref="AJ22:AL22"/>
+    <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AJ24:AN24"/>
+    <mergeCell ref="AJ17:AL17"/>
+    <mergeCell ref="AM17:AN17"/>
+    <mergeCell ref="AJ19:AN19"/>
+    <mergeCell ref="AJ20:AL20"/>
+    <mergeCell ref="AM20:AN20"/>
     <mergeCell ref="AJ32:AL32"/>
     <mergeCell ref="AM32:AN32"/>
     <mergeCell ref="S1:V2"/>
@@ -2414,41 +2445,6 @@
     <mergeCell ref="AM27:AN27"/>
     <mergeCell ref="AJ21:AL21"/>
     <mergeCell ref="AM21:AN21"/>
-    <mergeCell ref="AJ22:AL22"/>
-    <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="AJ24:AN24"/>
-    <mergeCell ref="AJ17:AL17"/>
-    <mergeCell ref="AM17:AN17"/>
-    <mergeCell ref="AJ19:AN19"/>
-    <mergeCell ref="AJ20:AL20"/>
-    <mergeCell ref="AM20:AN20"/>
-    <mergeCell ref="AJ14:AN14"/>
-    <mergeCell ref="AJ15:AL15"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="AJ16:AL16"/>
-    <mergeCell ref="AM16:AN16"/>
-    <mergeCell ref="AJ10:AL10"/>
-    <mergeCell ref="AM10:AN10"/>
-    <mergeCell ref="AJ11:AL11"/>
-    <mergeCell ref="AM11:AN11"/>
-    <mergeCell ref="AJ12:AL12"/>
-    <mergeCell ref="AM12:AN12"/>
-    <mergeCell ref="AJ6:AL6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="AJ9:AN9"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="AE3:AI3"/>
-    <mergeCell ref="AJ3:AN3"/>
-    <mergeCell ref="AJ4:AN4"/>
-    <mergeCell ref="AJ5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="U3:Y3"/>
   </mergeCells>
   <pageMargins left="0.389583333333333" right="0.389583333333333" top="1" bottom="0.58958333333333302" header="0.30972222222222201" footer="0.30972222222222201"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
#56828 has been resolved
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
@@ -26,11 +26,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,15 +45,46 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FFE2EFDA"/>
-      <name val="MS ゴシック"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -68,81 +99,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -159,7 +122,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,7 +130,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,27 +168,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,187 +204,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,16 +522,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,9 +547,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,52 +595,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -623,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -641,134 +641,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -811,31 +811,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,6 +860,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
@@ -910,6 +925,7 @@
     <mruColors>
       <color rgb="007F9698"/>
       <color rgb="00E2EFDA"/>
+      <color rgb="00DDDDD2"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1237,11 +1253,11 @@
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="4"/>
-      <c r="AJ3" s="23"/>
-      <c r="AK3" s="24"/>
-      <c r="AL3" s="24"/>
-      <c r="AM3" s="24"/>
-      <c r="AN3" s="25"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="29"/>
     </row>
     <row r="4" customHeight="1" spans="1:40">
       <c r="A4" s="5"/>
@@ -1279,11 +1295,11 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="7"/>
-      <c r="AJ4" s="26"/>
+      <c r="AJ4" s="30"/>
       <c r="AK4" s="13"/>
       <c r="AL4" s="13"/>
       <c r="AM4" s="13"/>
-      <c r="AN4" s="22"/>
+      <c r="AN4" s="31"/>
     </row>
     <row r="5" customHeight="1" spans="1:40">
       <c r="A5" s="8"/>
@@ -1376,9 +1392,9 @@
       <c r="AH8" s="11"/>
       <c r="AI8" s="12"/>
       <c r="AJ8" s="8"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="27"/>
-      <c r="AM8" s="27"/>
+      <c r="AK8" s="32"/>
+      <c r="AL8" s="32"/>
+      <c r="AM8" s="32"/>
       <c r="AN8" s="9"/>
     </row>
     <row r="9" customHeight="1" spans="1:40">
@@ -1511,9 +1527,9 @@
       <c r="AH13" s="11"/>
       <c r="AI13" s="12"/>
       <c r="AJ13" s="8"/>
-      <c r="AK13" s="27"/>
-      <c r="AL13" s="27"/>
-      <c r="AM13" s="27"/>
+      <c r="AK13" s="32"/>
+      <c r="AL13" s="32"/>
+      <c r="AM13" s="32"/>
       <c r="AN13" s="9"/>
     </row>
     <row r="14" customHeight="1" spans="1:40">
@@ -1646,9 +1662,9 @@
       <c r="AH18" s="11"/>
       <c r="AI18" s="12"/>
       <c r="AJ18" s="8"/>
-      <c r="AK18" s="27"/>
-      <c r="AL18" s="27"/>
-      <c r="AM18" s="27"/>
+      <c r="AK18" s="32"/>
+      <c r="AL18" s="32"/>
+      <c r="AM18" s="32"/>
       <c r="AN18" s="9"/>
     </row>
     <row r="19" customHeight="1" spans="1:40">
@@ -1781,9 +1797,9 @@
       <c r="AH23" s="11"/>
       <c r="AI23" s="12"/>
       <c r="AJ23" s="8"/>
-      <c r="AK23" s="27"/>
-      <c r="AL23" s="27"/>
-      <c r="AM23" s="27"/>
+      <c r="AK23" s="32"/>
+      <c r="AL23" s="32"/>
+      <c r="AM23" s="32"/>
       <c r="AN23" s="9"/>
     </row>
     <row r="24" customHeight="1" spans="1:40">
@@ -1916,9 +1932,9 @@
       <c r="AH28" s="11"/>
       <c r="AI28" s="12"/>
       <c r="AJ28" s="8"/>
-      <c r="AK28" s="27"/>
-      <c r="AL28" s="27"/>
-      <c r="AM28" s="27"/>
+      <c r="AK28" s="32"/>
+      <c r="AL28" s="32"/>
+      <c r="AM28" s="32"/>
       <c r="AN28" s="9"/>
     </row>
     <row r="29" customHeight="1" spans="1:40">
@@ -2081,7 +2097,7 @@
   <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3:AN3"/>
+      <selection activeCell="AJ33" sqref="AJ33:AN33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.13888888888889" defaultRowHeight="14.1" customHeight="1"/>
@@ -2205,8 +2221,8 @@
       <c r="AJ5" s="20"/>
       <c r="AK5" s="21"/>
       <c r="AL5" s="21"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="22"/>
+      <c r="AM5" s="22"/>
+      <c r="AN5" s="23"/>
     </row>
     <row r="6" customHeight="1" spans="1:40">
       <c r="A6" s="8"/>
@@ -2226,8 +2242,8 @@
       <c r="AJ6" s="20"/>
       <c r="AK6" s="21"/>
       <c r="AL6" s="21"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="22"/>
+      <c r="AM6" s="22"/>
+      <c r="AN6" s="23"/>
     </row>
     <row r="7" customHeight="1" spans="1:40">
       <c r="A7" s="8"/>
@@ -2247,8 +2263,8 @@
       <c r="AJ7" s="20"/>
       <c r="AK7" s="21"/>
       <c r="AL7" s="21"/>
-      <c r="AM7" s="13"/>
-      <c r="AN7" s="22"/>
+      <c r="AM7" s="22"/>
+      <c r="AN7" s="23"/>
     </row>
     <row r="8" customHeight="1" spans="1:40">
       <c r="A8" s="10"/>
@@ -2286,11 +2302,11 @@
       <c r="AG8" s="11"/>
       <c r="AH8" s="11"/>
       <c r="AI8" s="12"/>
-      <c r="AJ8" s="10"/>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="12"/>
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="25"/>
+      <c r="AL8" s="25"/>
+      <c r="AM8" s="25"/>
+      <c r="AN8" s="26"/>
     </row>
     <row r="9" customHeight="1" spans="1:40">
       <c r="A9" s="5"/>
@@ -2352,8 +2368,8 @@
       <c r="AJ10" s="20"/>
       <c r="AK10" s="21"/>
       <c r="AL10" s="21"/>
-      <c r="AM10" s="13"/>
-      <c r="AN10" s="22"/>
+      <c r="AM10" s="22"/>
+      <c r="AN10" s="23"/>
     </row>
     <row r="11" customHeight="1" spans="1:40">
       <c r="A11" s="8"/>
@@ -2373,8 +2389,8 @@
       <c r="AJ11" s="20"/>
       <c r="AK11" s="21"/>
       <c r="AL11" s="21"/>
-      <c r="AM11" s="13"/>
-      <c r="AN11" s="22"/>
+      <c r="AM11" s="22"/>
+      <c r="AN11" s="23"/>
     </row>
     <row r="12" customHeight="1" spans="1:40">
       <c r="A12" s="8"/>
@@ -2394,8 +2410,8 @@
       <c r="AJ12" s="20"/>
       <c r="AK12" s="21"/>
       <c r="AL12" s="21"/>
-      <c r="AM12" s="13"/>
-      <c r="AN12" s="22"/>
+      <c r="AM12" s="22"/>
+      <c r="AN12" s="23"/>
     </row>
     <row r="13" customHeight="1" spans="1:40">
       <c r="A13" s="10"/>
@@ -2433,11 +2449,11 @@
       <c r="AG13" s="11"/>
       <c r="AH13" s="11"/>
       <c r="AI13" s="12"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="12"/>
+      <c r="AJ13" s="24"/>
+      <c r="AK13" s="25"/>
+      <c r="AL13" s="25"/>
+      <c r="AM13" s="25"/>
+      <c r="AN13" s="26"/>
     </row>
     <row r="14" customHeight="1" spans="1:40">
       <c r="A14" s="5"/>
@@ -2499,8 +2515,8 @@
       <c r="AJ15" s="20"/>
       <c r="AK15" s="21"/>
       <c r="AL15" s="21"/>
-      <c r="AM15" s="13"/>
-      <c r="AN15" s="22"/>
+      <c r="AM15" s="22"/>
+      <c r="AN15" s="23"/>
     </row>
     <row r="16" customHeight="1" spans="1:40">
       <c r="A16" s="8"/>
@@ -2520,8 +2536,8 @@
       <c r="AJ16" s="20"/>
       <c r="AK16" s="21"/>
       <c r="AL16" s="21"/>
-      <c r="AM16" s="13"/>
-      <c r="AN16" s="22"/>
+      <c r="AM16" s="22"/>
+      <c r="AN16" s="23"/>
     </row>
     <row r="17" customHeight="1" spans="1:40">
       <c r="A17" s="8"/>
@@ -2541,8 +2557,8 @@
       <c r="AJ17" s="20"/>
       <c r="AK17" s="21"/>
       <c r="AL17" s="21"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="22"/>
+      <c r="AM17" s="22"/>
+      <c r="AN17" s="23"/>
     </row>
     <row r="18" customHeight="1" spans="1:40">
       <c r="A18" s="10"/>
@@ -2580,11 +2596,11 @@
       <c r="AG18" s="11"/>
       <c r="AH18" s="11"/>
       <c r="AI18" s="12"/>
-      <c r="AJ18" s="10"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="11"/>
-      <c r="AN18" s="12"/>
+      <c r="AJ18" s="24"/>
+      <c r="AK18" s="25"/>
+      <c r="AL18" s="25"/>
+      <c r="AM18" s="25"/>
+      <c r="AN18" s="26"/>
     </row>
     <row r="19" customHeight="1" spans="1:40">
       <c r="A19" s="5"/>
@@ -2646,8 +2662,8 @@
       <c r="AJ20" s="20"/>
       <c r="AK20" s="21"/>
       <c r="AL20" s="21"/>
-      <c r="AM20" s="13"/>
-      <c r="AN20" s="22"/>
+      <c r="AM20" s="22"/>
+      <c r="AN20" s="23"/>
     </row>
     <row r="21" customHeight="1" spans="1:40">
       <c r="A21" s="8"/>
@@ -2667,8 +2683,8 @@
       <c r="AJ21" s="20"/>
       <c r="AK21" s="21"/>
       <c r="AL21" s="21"/>
-      <c r="AM21" s="13"/>
-      <c r="AN21" s="22"/>
+      <c r="AM21" s="22"/>
+      <c r="AN21" s="23"/>
     </row>
     <row r="22" customHeight="1" spans="1:40">
       <c r="A22" s="8"/>
@@ -2688,8 +2704,8 @@
       <c r="AJ22" s="20"/>
       <c r="AK22" s="21"/>
       <c r="AL22" s="21"/>
-      <c r="AM22" s="13"/>
-      <c r="AN22" s="22"/>
+      <c r="AM22" s="22"/>
+      <c r="AN22" s="23"/>
     </row>
     <row r="23" customHeight="1" spans="1:40">
       <c r="A23" s="10"/>
@@ -2727,11 +2743,11 @@
       <c r="AG23" s="11"/>
       <c r="AH23" s="11"/>
       <c r="AI23" s="12"/>
-      <c r="AJ23" s="10"/>
-      <c r="AK23" s="11"/>
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="11"/>
-      <c r="AN23" s="12"/>
+      <c r="AJ23" s="24"/>
+      <c r="AK23" s="25"/>
+      <c r="AL23" s="25"/>
+      <c r="AM23" s="25"/>
+      <c r="AN23" s="26"/>
     </row>
     <row r="24" customHeight="1" spans="1:40">
       <c r="A24" s="5"/>
@@ -2793,8 +2809,8 @@
       <c r="AJ25" s="20"/>
       <c r="AK25" s="21"/>
       <c r="AL25" s="21"/>
-      <c r="AM25" s="13"/>
-      <c r="AN25" s="22"/>
+      <c r="AM25" s="22"/>
+      <c r="AN25" s="23"/>
     </row>
     <row r="26" customHeight="1" spans="1:40">
       <c r="A26" s="8"/>
@@ -2814,8 +2830,8 @@
       <c r="AJ26" s="20"/>
       <c r="AK26" s="21"/>
       <c r="AL26" s="21"/>
-      <c r="AM26" s="13"/>
-      <c r="AN26" s="22"/>
+      <c r="AM26" s="22"/>
+      <c r="AN26" s="23"/>
     </row>
     <row r="27" customHeight="1" spans="1:40">
       <c r="A27" s="8"/>
@@ -2835,8 +2851,8 @@
       <c r="AJ27" s="20"/>
       <c r="AK27" s="21"/>
       <c r="AL27" s="21"/>
-      <c r="AM27" s="13"/>
-      <c r="AN27" s="22"/>
+      <c r="AM27" s="22"/>
+      <c r="AN27" s="23"/>
     </row>
     <row r="28" customHeight="1" spans="1:40">
       <c r="A28" s="10"/>
@@ -2874,11 +2890,11 @@
       <c r="AG28" s="11"/>
       <c r="AH28" s="11"/>
       <c r="AI28" s="12"/>
-      <c r="AJ28" s="10"/>
-      <c r="AK28" s="11"/>
-      <c r="AL28" s="11"/>
-      <c r="AM28" s="11"/>
-      <c r="AN28" s="12"/>
+      <c r="AJ28" s="24"/>
+      <c r="AK28" s="25"/>
+      <c r="AL28" s="25"/>
+      <c r="AM28" s="25"/>
+      <c r="AN28" s="26"/>
     </row>
     <row r="29" customHeight="1" spans="1:40">
       <c r="A29" s="5"/>
@@ -2940,8 +2956,8 @@
       <c r="AJ30" s="20"/>
       <c r="AK30" s="21"/>
       <c r="AL30" s="21"/>
-      <c r="AM30" s="13"/>
-      <c r="AN30" s="22"/>
+      <c r="AM30" s="22"/>
+      <c r="AN30" s="23"/>
     </row>
     <row r="31" customHeight="1" spans="1:40">
       <c r="A31" s="8"/>
@@ -2961,8 +2977,8 @@
       <c r="AJ31" s="20"/>
       <c r="AK31" s="21"/>
       <c r="AL31" s="21"/>
-      <c r="AM31" s="13"/>
-      <c r="AN31" s="22"/>
+      <c r="AM31" s="22"/>
+      <c r="AN31" s="23"/>
     </row>
     <row r="32" customHeight="1" spans="1:40">
       <c r="A32" s="8"/>
@@ -2982,8 +2998,8 @@
       <c r="AJ32" s="20"/>
       <c r="AK32" s="21"/>
       <c r="AL32" s="21"/>
-      <c r="AM32" s="13"/>
-      <c r="AN32" s="22"/>
+      <c r="AM32" s="22"/>
+      <c r="AN32" s="23"/>
     </row>
     <row r="33" customHeight="1" spans="1:40">
       <c r="A33" s="10"/>
@@ -3021,14 +3037,14 @@
       <c r="AG33" s="11"/>
       <c r="AH33" s="11"/>
       <c r="AI33" s="12"/>
-      <c r="AJ33" s="10"/>
-      <c r="AK33" s="11"/>
-      <c r="AL33" s="11"/>
-      <c r="AM33" s="11"/>
-      <c r="AN33" s="12"/>
+      <c r="AJ33" s="24"/>
+      <c r="AK33" s="25"/>
+      <c r="AL33" s="25"/>
+      <c r="AM33" s="25"/>
+      <c r="AN33" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="51">
+  <mergeCells count="57">
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="K3:O3"/>
@@ -3044,6 +3060,7 @@
     <mergeCell ref="AM6:AN6"/>
     <mergeCell ref="AJ7:AL7"/>
     <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="AJ8:AN8"/>
     <mergeCell ref="AJ9:AN9"/>
     <mergeCell ref="AJ10:AL10"/>
     <mergeCell ref="AM10:AN10"/>
@@ -3051,6 +3068,7 @@
     <mergeCell ref="AM11:AN11"/>
     <mergeCell ref="AJ12:AL12"/>
     <mergeCell ref="AM12:AN12"/>
+    <mergeCell ref="AJ13:AN13"/>
     <mergeCell ref="AJ14:AN14"/>
     <mergeCell ref="AJ15:AL15"/>
     <mergeCell ref="AM15:AN15"/>
@@ -3058,6 +3076,7 @@
     <mergeCell ref="AM16:AN16"/>
     <mergeCell ref="AJ17:AL17"/>
     <mergeCell ref="AM17:AN17"/>
+    <mergeCell ref="AJ18:AN18"/>
     <mergeCell ref="AJ19:AN19"/>
     <mergeCell ref="AJ20:AL20"/>
     <mergeCell ref="AM20:AN20"/>
@@ -3065,6 +3084,7 @@
     <mergeCell ref="AM21:AN21"/>
     <mergeCell ref="AJ22:AL22"/>
     <mergeCell ref="AM22:AN22"/>
+    <mergeCell ref="AJ23:AN23"/>
     <mergeCell ref="AJ24:AN24"/>
     <mergeCell ref="AJ25:AL25"/>
     <mergeCell ref="AM25:AN25"/>
@@ -3072,6 +3092,7 @@
     <mergeCell ref="AM26:AN26"/>
     <mergeCell ref="AJ27:AL27"/>
     <mergeCell ref="AM27:AN27"/>
+    <mergeCell ref="AJ28:AN28"/>
     <mergeCell ref="AJ29:AN29"/>
     <mergeCell ref="AJ30:AL30"/>
     <mergeCell ref="AM30:AN30"/>
@@ -3079,6 +3100,7 @@
     <mergeCell ref="AM31:AN31"/>
     <mergeCell ref="AJ32:AL32"/>
     <mergeCell ref="AM32:AN32"/>
+    <mergeCell ref="AJ33:AN33"/>
     <mergeCell ref="S1:V2"/>
   </mergeCells>
   <pageMargins left="0.389583333333333" right="0.389583333333333" top="1" bottom="0.589583333333333" header="0.309722222222222" footer="0.309722222222222"/>

</xml_diff>

<commit_message>
ksu002B has been resolved
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KSU002B.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="テンプレート  " sheetId="2" r:id="rId1"/>
@@ -28,10 +28,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -49,15 +49,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -68,21 +81,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -103,29 +101,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -134,44 +109,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,7 +133,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,13 +201,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDD2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,7 +291,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,67 +327,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,13 +339,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,55 +357,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,13 +369,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,41 +548,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,13 +574,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,157 +606,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -796,18 +796,72 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,54 +870,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -934,6 +940,7 @@
     <mruColors>
       <color rgb="007F9698"/>
       <color rgb="00E2EFDA"/>
+      <color rgb="00808080"/>
       <color rgb="00DDDDD2"/>
     </mruColors>
   </colors>
@@ -1205,7 +1212,7 @@
   <sheetPr/>
   <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1215,16 +1222,16 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="19:22">
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" customHeight="1" spans="19:22">
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
     </row>
     <row r="3" customHeight="1" spans="1:40">
       <c r="A3" s="2"/>
@@ -1318,142 +1325,170 @@
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="7"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="12"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="30"/>
     </row>
     <row r="5" customHeight="1" spans="1:40">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="11"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="11"/>
       <c r="K5" s="8"/>
       <c r="L5" s="9"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="11"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="9"/>
-      <c r="S5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="9"/>
       <c r="T5" s="11"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9"/>
-      <c r="X5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="9"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="9"/>
-      <c r="AC5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="9"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="8"/>
       <c r="AF5" s="9"/>
-      <c r="AH5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="9"/>
       <c r="AI5" s="11"/>
-      <c r="AJ5" s="13"/>
-      <c r="AN5" s="14"/>
+      <c r="AJ5" s="31"/>
+      <c r="AN5" s="32"/>
     </row>
     <row r="6" customHeight="1" spans="1:40">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="8"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="12"/>
+      <c r="O6" s="11"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="12"/>
+      <c r="T6" s="11"/>
       <c r="U6" s="8"/>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="Y6" s="12"/>
+      <c r="Y6" s="11"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="12"/>
+      <c r="AD6" s="11"/>
       <c r="AE6" s="8"/>
       <c r="AF6" s="9"/>
       <c r="AG6" s="9"/>
       <c r="AH6" s="9"/>
-      <c r="AI6" s="12"/>
-      <c r="AJ6" s="13"/>
-      <c r="AN6" s="14"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="31"/>
+      <c r="AN6" s="32"/>
     </row>
     <row r="7" customHeight="1" spans="1:40">
-      <c r="A7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="13"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="13"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="13"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="13"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="13"/>
-      <c r="AI7" s="14"/>
-      <c r="AJ7" s="13"/>
-      <c r="AN7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="31"/>
+      <c r="AN7" s="32"/>
     </row>
     <row r="8" customHeight="1" spans="1:40">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="17"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="17"/>
-      <c r="AJ8" s="13"/>
-      <c r="AK8" s="31"/>
-      <c r="AL8" s="31"/>
-      <c r="AM8" s="31"/>
-      <c r="AN8" s="14"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="31"/>
+      <c r="AK8" s="33"/>
+      <c r="AL8" s="33"/>
+      <c r="AM8" s="33"/>
+      <c r="AN8" s="32"/>
     </row>
     <row r="9" customHeight="1" spans="1:40">
       <c r="A9" s="5" t="s">
@@ -1505,139 +1540,167 @@
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="7"/>
-      <c r="AJ9" s="13"/>
-      <c r="AN9" s="14"/>
+      <c r="AJ9" s="31"/>
+      <c r="AN9" s="32"/>
     </row>
     <row r="10" customHeight="1" spans="1:40">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="11"/>
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="9"/>
       <c r="O10" s="11"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="9"/>
-      <c r="S10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="11"/>
       <c r="U10" s="8"/>
       <c r="V10" s="9"/>
-      <c r="X10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="9"/>
       <c r="Y10" s="11"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="9"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="9"/>
       <c r="AD10" s="11"/>
       <c r="AE10" s="8"/>
       <c r="AF10" s="9"/>
-      <c r="AH10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="9"/>
       <c r="AI10" s="11"/>
-      <c r="AJ10" s="13"/>
-      <c r="AN10" s="14"/>
+      <c r="AJ10" s="31"/>
+      <c r="AN10" s="32"/>
     </row>
     <row r="11" customHeight="1" spans="1:40">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="8"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="12"/>
+      <c r="O11" s="11"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="12"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="8"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="Y11" s="12"/>
+      <c r="Y11" s="11"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
-      <c r="AD11" s="12"/>
+      <c r="AD11" s="11"/>
       <c r="AE11" s="8"/>
       <c r="AF11" s="9"/>
       <c r="AG11" s="9"/>
       <c r="AH11" s="9"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="13"/>
-      <c r="AN11" s="14"/>
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="31"/>
+      <c r="AN11" s="32"/>
     </row>
     <row r="12" customHeight="1" spans="1:40">
-      <c r="A12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="13"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="13"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="13"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="13"/>
-      <c r="AI12" s="14"/>
-      <c r="AJ12" s="13"/>
-      <c r="AN12" s="14"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="31"/>
+      <c r="AN12" s="32"/>
     </row>
     <row r="13" customHeight="1" spans="1:40">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="17"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="17"/>
-      <c r="AJ13" s="13"/>
-      <c r="AK13" s="31"/>
-      <c r="AL13" s="31"/>
-      <c r="AM13" s="31"/>
-      <c r="AN13" s="14"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="31"/>
+      <c r="AK13" s="33"/>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="33"/>
+      <c r="AN13" s="32"/>
     </row>
     <row r="14" customHeight="1" spans="1:40">
       <c r="A14" s="5" t="s">
@@ -1689,139 +1752,167 @@
       <c r="AG14" s="6"/>
       <c r="AH14" s="6"/>
       <c r="AI14" s="7"/>
-      <c r="AJ14" s="13"/>
-      <c r="AN14" s="14"/>
+      <c r="AJ14" s="31"/>
+      <c r="AN14" s="32"/>
     </row>
     <row r="15" customHeight="1" spans="1:40">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="11"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
-      <c r="I15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="11"/>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
-      <c r="N15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="9"/>
       <c r="O15" s="11"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
-      <c r="S15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="9"/>
       <c r="T15" s="11"/>
       <c r="U15" s="8"/>
       <c r="V15" s="9"/>
-      <c r="X15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="9"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="9"/>
-      <c r="AC15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="9"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="8"/>
       <c r="AF15" s="9"/>
-      <c r="AH15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="9"/>
       <c r="AI15" s="11"/>
-      <c r="AJ15" s="13"/>
-      <c r="AN15" s="14"/>
+      <c r="AJ15" s="31"/>
+      <c r="AN15" s="32"/>
     </row>
     <row r="16" customHeight="1" spans="1:40">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="12"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="8"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="12"/>
+      <c r="O16" s="11"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="12"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="8"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
-      <c r="Y16" s="12"/>
+      <c r="Y16" s="11"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
-      <c r="AD16" s="12"/>
+      <c r="AD16" s="11"/>
       <c r="AE16" s="8"/>
       <c r="AF16" s="9"/>
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
-      <c r="AI16" s="12"/>
-      <c r="AJ16" s="13"/>
-      <c r="AN16" s="14"/>
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="31"/>
+      <c r="AN16" s="32"/>
     </row>
     <row r="17" customHeight="1" spans="1:40">
-      <c r="A17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="13"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="13"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="13"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="13"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="13"/>
-      <c r="AI17" s="14"/>
-      <c r="AJ17" s="13"/>
-      <c r="AN17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="31"/>
+      <c r="AN17" s="32"/>
     </row>
     <row r="18" customHeight="1" spans="1:40">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="17"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="16"/>
-      <c r="AG18" s="16"/>
-      <c r="AH18" s="16"/>
-      <c r="AI18" s="17"/>
-      <c r="AJ18" s="13"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
-      <c r="AM18" s="31"/>
-      <c r="AN18" s="14"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="16"/>
+      <c r="AJ18" s="31"/>
+      <c r="AK18" s="33"/>
+      <c r="AL18" s="33"/>
+      <c r="AM18" s="33"/>
+      <c r="AN18" s="32"/>
     </row>
     <row r="19" customHeight="1" spans="1:40">
       <c r="A19" s="5" t="s">
@@ -1873,139 +1964,167 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="6"/>
       <c r="AI19" s="7"/>
-      <c r="AJ19" s="13"/>
-      <c r="AN19" s="14"/>
+      <c r="AJ19" s="31"/>
+      <c r="AN19" s="32"/>
     </row>
     <row r="20" customHeight="1" spans="1:40">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="11"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
-      <c r="I20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="11"/>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
-      <c r="N20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="9"/>
       <c r="O20" s="11"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
-      <c r="S20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="9"/>
       <c r="T20" s="11"/>
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
-      <c r="X20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="9"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="8"/>
       <c r="AA20" s="9"/>
-      <c r="AC20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="9"/>
       <c r="AD20" s="11"/>
       <c r="AE20" s="8"/>
       <c r="AF20" s="9"/>
-      <c r="AH20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="9"/>
       <c r="AI20" s="11"/>
-      <c r="AJ20" s="13"/>
-      <c r="AN20" s="14"/>
+      <c r="AJ20" s="31"/>
+      <c r="AN20" s="32"/>
     </row>
     <row r="21" customHeight="1" spans="1:40">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="8"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="12"/>
+      <c r="J21" s="11"/>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="11"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="12"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="8"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
-      <c r="Y21" s="12"/>
+      <c r="Y21" s="11"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
-      <c r="AD21" s="12"/>
+      <c r="AD21" s="11"/>
       <c r="AE21" s="8"/>
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="9"/>
-      <c r="AI21" s="12"/>
-      <c r="AJ21" s="13"/>
-      <c r="AN21" s="14"/>
+      <c r="AI21" s="11"/>
+      <c r="AJ21" s="31"/>
+      <c r="AN21" s="32"/>
     </row>
     <row r="22" customHeight="1" spans="1:40">
-      <c r="A22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="13"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="13"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="13"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="13"/>
-      <c r="AD22" s="14"/>
-      <c r="AE22" s="13"/>
-      <c r="AI22" s="14"/>
-      <c r="AJ22" s="13"/>
-      <c r="AN22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="12"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="13"/>
+      <c r="AJ22" s="31"/>
+      <c r="AN22" s="32"/>
     </row>
     <row r="23" customHeight="1" spans="1:40">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="16"/>
-      <c r="AD23" s="17"/>
-      <c r="AE23" s="15"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="16"/>
-      <c r="AH23" s="16"/>
-      <c r="AI23" s="17"/>
-      <c r="AJ23" s="13"/>
-      <c r="AK23" s="31"/>
-      <c r="AL23" s="31"/>
-      <c r="AM23" s="31"/>
-      <c r="AN23" s="14"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="31"/>
+      <c r="AK23" s="33"/>
+      <c r="AL23" s="33"/>
+      <c r="AM23" s="33"/>
+      <c r="AN23" s="32"/>
     </row>
     <row r="24" customHeight="1" spans="1:40">
       <c r="A24" s="5" t="s">
@@ -2057,139 +2176,167 @@
       <c r="AG24" s="6"/>
       <c r="AH24" s="6"/>
       <c r="AI24" s="7"/>
-      <c r="AJ24" s="13"/>
-      <c r="AN24" s="14"/>
+      <c r="AJ24" s="31"/>
+      <c r="AN24" s="32"/>
     </row>
     <row r="25" customHeight="1" spans="1:40">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="11"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="I25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="11"/>
       <c r="K25" s="8"/>
       <c r="L25" s="9"/>
-      <c r="N25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="9"/>
       <c r="O25" s="11"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
-      <c r="S25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="9"/>
       <c r="T25" s="11"/>
       <c r="U25" s="8"/>
       <c r="V25" s="9"/>
-      <c r="X25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="9"/>
       <c r="Y25" s="11"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="9"/>
-      <c r="AC25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="9"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="8"/>
       <c r="AF25" s="9"/>
-      <c r="AH25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="9"/>
       <c r="AI25" s="11"/>
-      <c r="AJ25" s="13"/>
-      <c r="AN25" s="14"/>
+      <c r="AJ25" s="31"/>
+      <c r="AN25" s="32"/>
     </row>
     <row r="26" customHeight="1" spans="1:40">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="12"/>
+      <c r="J26" s="11"/>
       <c r="K26" s="8"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="12"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="12"/>
+      <c r="T26" s="11"/>
       <c r="U26" s="8"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
-      <c r="Y26" s="12"/>
+      <c r="Y26" s="11"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AD26" s="12"/>
+      <c r="AD26" s="11"/>
       <c r="AE26" s="8"/>
       <c r="AF26" s="9"/>
       <c r="AG26" s="9"/>
       <c r="AH26" s="9"/>
-      <c r="AI26" s="12"/>
-      <c r="AJ26" s="13"/>
-      <c r="AN26" s="14"/>
+      <c r="AI26" s="11"/>
+      <c r="AJ26" s="31"/>
+      <c r="AN26" s="32"/>
     </row>
     <row r="27" customHeight="1" spans="1:40">
-      <c r="A27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="13"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="13"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="13"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="13"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="13"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="13"/>
-      <c r="AI27" s="14"/>
-      <c r="AJ27" s="13"/>
-      <c r="AN27" s="14"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="13"/>
+      <c r="AJ27" s="31"/>
+      <c r="AN27" s="32"/>
     </row>
     <row r="28" customHeight="1" spans="1:40">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
-      <c r="AI28" s="17"/>
-      <c r="AJ28" s="13"/>
-      <c r="AK28" s="31"/>
-      <c r="AL28" s="31"/>
-      <c r="AM28" s="31"/>
-      <c r="AN28" s="14"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="16"/>
+      <c r="AJ28" s="31"/>
+      <c r="AK28" s="33"/>
+      <c r="AL28" s="33"/>
+      <c r="AM28" s="33"/>
+      <c r="AN28" s="32"/>
     </row>
     <row r="29" customHeight="1" spans="1:40">
       <c r="A29" s="5" t="s">
@@ -2241,139 +2388,167 @@
       <c r="AG29" s="6"/>
       <c r="AH29" s="6"/>
       <c r="AI29" s="7"/>
-      <c r="AJ29" s="13"/>
-      <c r="AN29" s="14"/>
+      <c r="AJ29" s="31"/>
+      <c r="AN29" s="32"/>
     </row>
     <row r="30" customHeight="1" spans="1:40">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="11"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
-      <c r="I30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="11"/>
       <c r="K30" s="8"/>
       <c r="L30" s="9"/>
-      <c r="N30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="9"/>
       <c r="O30" s="11"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="9"/>
-      <c r="S30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="9"/>
       <c r="T30" s="11"/>
       <c r="U30" s="8"/>
       <c r="V30" s="9"/>
-      <c r="X30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="9"/>
       <c r="Y30" s="11"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="9"/>
-      <c r="AC30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="9"/>
       <c r="AD30" s="11"/>
       <c r="AE30" s="8"/>
       <c r="AF30" s="9"/>
-      <c r="AH30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="9"/>
       <c r="AI30" s="11"/>
-      <c r="AJ30" s="13"/>
-      <c r="AN30" s="14"/>
+      <c r="AJ30" s="31"/>
+      <c r="AN30" s="32"/>
     </row>
     <row r="31" customHeight="1" spans="1:40">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="12"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="12"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="8"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="12"/>
+      <c r="O31" s="11"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
-      <c r="T31" s="12"/>
+      <c r="T31" s="11"/>
       <c r="U31" s="8"/>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
-      <c r="Y31" s="12"/>
+      <c r="Y31" s="11"/>
       <c r="Z31" s="8"/>
       <c r="AA31" s="9"/>
       <c r="AB31" s="9"/>
       <c r="AC31" s="9"/>
-      <c r="AD31" s="12"/>
+      <c r="AD31" s="11"/>
       <c r="AE31" s="8"/>
       <c r="AF31" s="9"/>
       <c r="AG31" s="9"/>
       <c r="AH31" s="9"/>
-      <c r="AI31" s="12"/>
-      <c r="AJ31" s="13"/>
-      <c r="AN31" s="14"/>
+      <c r="AI31" s="11"/>
+      <c r="AJ31" s="31"/>
+      <c r="AN31" s="32"/>
     </row>
     <row r="32" customHeight="1" spans="1:40">
-      <c r="A32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="13"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="13"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="13"/>
-      <c r="Y32" s="14"/>
-      <c r="Z32" s="13"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="13"/>
-      <c r="AI32" s="14"/>
-      <c r="AJ32" s="13"/>
-      <c r="AN32" s="14"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="31"/>
+      <c r="AN32" s="32"/>
     </row>
     <row r="33" customHeight="1" spans="1:40">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="16"/>
-      <c r="X33" s="16"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="16"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="15"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="16"/>
-      <c r="AH33" s="16"/>
-      <c r="AI33" s="17"/>
-      <c r="AJ33" s="32"/>
-      <c r="AK33" s="33"/>
-      <c r="AL33" s="33"/>
-      <c r="AM33" s="33"/>
-      <c r="AN33" s="34"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="34"/>
+      <c r="AK33" s="35"/>
+      <c r="AL33" s="35"/>
+      <c r="AM33" s="35"/>
+      <c r="AN33" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="220">
@@ -2414,13 +2589,6 @@
     <mergeCell ref="U6:Y6"/>
     <mergeCell ref="Z6:AD6"/>
     <mergeCell ref="AE6:AI6"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="U8:Y8"/>
-    <mergeCell ref="Z8:AD8"/>
-    <mergeCell ref="AE8:AI8"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="K9:O9"/>
@@ -2449,13 +2617,6 @@
     <mergeCell ref="U11:Y11"/>
     <mergeCell ref="Z11:AD11"/>
     <mergeCell ref="AE11:AI11"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="P13:T13"/>
-    <mergeCell ref="U13:Y13"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="AE13:AI13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="K14:O14"/>
@@ -2484,13 +2645,6 @@
     <mergeCell ref="U16:Y16"/>
     <mergeCell ref="Z16:AD16"/>
     <mergeCell ref="AE16:AI16"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="P18:T18"/>
-    <mergeCell ref="U18:Y18"/>
-    <mergeCell ref="Z18:AD18"/>
-    <mergeCell ref="AE18:AI18"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="F19:J19"/>
     <mergeCell ref="K19:O19"/>
@@ -2519,13 +2673,6 @@
     <mergeCell ref="U21:Y21"/>
     <mergeCell ref="Z21:AD21"/>
     <mergeCell ref="AE21:AI21"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:Y23"/>
-    <mergeCell ref="Z23:AD23"/>
-    <mergeCell ref="AE23:AI23"/>
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="F24:J24"/>
     <mergeCell ref="K24:O24"/>
@@ -2554,13 +2701,6 @@
     <mergeCell ref="U26:Y26"/>
     <mergeCell ref="Z26:AD26"/>
     <mergeCell ref="AE26:AI26"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="U28:Y28"/>
-    <mergeCell ref="Z28:AD28"/>
-    <mergeCell ref="AE28:AI28"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="F29:J29"/>
     <mergeCell ref="K29:O29"/>
@@ -2589,14 +2729,49 @@
     <mergeCell ref="U31:Y31"/>
     <mergeCell ref="Z31:AD31"/>
     <mergeCell ref="AE31:AI31"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="K33:O33"/>
-    <mergeCell ref="P33:T33"/>
-    <mergeCell ref="U33:Y33"/>
-    <mergeCell ref="Z33:AD33"/>
-    <mergeCell ref="AE33:AI33"/>
     <mergeCell ref="S1:V2"/>
+    <mergeCell ref="A7:E8"/>
+    <mergeCell ref="F7:J8"/>
+    <mergeCell ref="K7:O8"/>
+    <mergeCell ref="P7:T8"/>
+    <mergeCell ref="U7:Y8"/>
+    <mergeCell ref="Z7:AD8"/>
+    <mergeCell ref="AE7:AI8"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:J13"/>
+    <mergeCell ref="K12:O13"/>
+    <mergeCell ref="P12:T13"/>
+    <mergeCell ref="U12:Y13"/>
+    <mergeCell ref="Z12:AD13"/>
+    <mergeCell ref="AE12:AI13"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="F17:J18"/>
+    <mergeCell ref="K17:O18"/>
+    <mergeCell ref="P17:T18"/>
+    <mergeCell ref="U17:Y18"/>
+    <mergeCell ref="Z17:AD18"/>
+    <mergeCell ref="AE17:AI18"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="F22:J23"/>
+    <mergeCell ref="K22:O23"/>
+    <mergeCell ref="P22:T23"/>
+    <mergeCell ref="U22:Y23"/>
+    <mergeCell ref="Z22:AD23"/>
+    <mergeCell ref="AE22:AI23"/>
+    <mergeCell ref="A27:E28"/>
+    <mergeCell ref="F27:J28"/>
+    <mergeCell ref="K27:O28"/>
+    <mergeCell ref="P27:T28"/>
+    <mergeCell ref="U27:Y28"/>
+    <mergeCell ref="Z27:AD28"/>
+    <mergeCell ref="AE27:AI28"/>
+    <mergeCell ref="A32:E33"/>
+    <mergeCell ref="F32:J33"/>
+    <mergeCell ref="K32:O33"/>
+    <mergeCell ref="P32:T33"/>
+    <mergeCell ref="U32:Y33"/>
+    <mergeCell ref="Z32:AD33"/>
+    <mergeCell ref="AE32:AI33"/>
   </mergeCells>
   <pageMargins left="0.389583333333333" right="0.389583333333333" top="1" bottom="0.589583333333333" header="0.309722222222222" footer="0.309722222222222"/>
   <pageSetup paperSize="1" orientation="landscape" horizontalDpi="600"/>
@@ -2609,7 +2784,7 @@
   <sheetPr/>
   <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2619,16 +2794,16 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="19:22">
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" customHeight="1" spans="19:22">
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
     </row>
     <row r="3" customHeight="1" spans="1:40">
       <c r="A3" s="2"/>
@@ -2733,142 +2908,170 @@
     <row r="5" customHeight="1" spans="1:40">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="11"/>
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="11"/>
       <c r="K5" s="8"/>
       <c r="L5" s="9"/>
-      <c r="N5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="9"/>
       <c r="O5" s="11"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="9"/>
-      <c r="S5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="9"/>
       <c r="T5" s="11"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9"/>
-      <c r="X5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="9"/>
       <c r="Y5" s="11"/>
       <c r="Z5" s="8"/>
       <c r="AA5" s="9"/>
-      <c r="AC5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="9"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="8"/>
       <c r="AF5" s="9"/>
-      <c r="AH5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="9"/>
       <c r="AI5" s="11"/>
       <c r="AJ5" s="24"/>
       <c r="AK5" s="25"/>
       <c r="AL5" s="25"/>
-      <c r="AM5" s="26"/>
-      <c r="AN5" s="27"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="11"/>
     </row>
     <row r="6" customHeight="1" spans="1:40">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="12"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="8"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="12"/>
+      <c r="O6" s="11"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
-      <c r="T6" s="12"/>
+      <c r="T6" s="11"/>
       <c r="U6" s="8"/>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
       <c r="X6" s="9"/>
-      <c r="Y6" s="12"/>
+      <c r="Y6" s="11"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9"/>
       <c r="AC6" s="9"/>
-      <c r="AD6" s="12"/>
+      <c r="AD6" s="11"/>
       <c r="AE6" s="8"/>
       <c r="AF6" s="9"/>
       <c r="AG6" s="9"/>
       <c r="AH6" s="9"/>
-      <c r="AI6" s="12"/>
+      <c r="AI6" s="11"/>
       <c r="AJ6" s="24"/>
       <c r="AK6" s="25"/>
       <c r="AL6" s="25"/>
-      <c r="AM6" s="26"/>
-      <c r="AN6" s="27"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="11"/>
     </row>
     <row r="7" customHeight="1" spans="1:40">
-      <c r="A7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="13"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="13"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="13"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="13"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="13"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="13"/>
-      <c r="AI7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="13"/>
       <c r="AJ7" s="24"/>
       <c r="AK7" s="25"/>
       <c r="AL7" s="25"/>
-      <c r="AM7" s="26"/>
-      <c r="AN7" s="27"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="11"/>
     </row>
     <row r="8" customHeight="1" spans="1:40">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="17"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="16"/>
-      <c r="AH8" s="16"/>
-      <c r="AI8" s="17"/>
-      <c r="AJ8" s="28"/>
-      <c r="AK8" s="29"/>
-      <c r="AL8" s="29"/>
-      <c r="AM8" s="29"/>
-      <c r="AN8" s="30"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15"/>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="26"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="28"/>
     </row>
     <row r="9" customHeight="1" spans="1:40">
       <c r="A9" s="5" t="s">
@@ -2929,142 +3132,170 @@
     <row r="10" customHeight="1" spans="1:40">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="11"/>
       <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="11"/>
       <c r="K10" s="8"/>
       <c r="L10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="9"/>
       <c r="O10" s="11"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="9"/>
-      <c r="S10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="11"/>
       <c r="U10" s="8"/>
       <c r="V10" s="9"/>
-      <c r="X10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="9"/>
       <c r="Y10" s="11"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="9"/>
-      <c r="AC10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="9"/>
       <c r="AD10" s="11"/>
       <c r="AE10" s="8"/>
       <c r="AF10" s="9"/>
-      <c r="AH10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="9"/>
       <c r="AI10" s="11"/>
       <c r="AJ10" s="24"/>
       <c r="AK10" s="25"/>
       <c r="AL10" s="25"/>
-      <c r="AM10" s="26"/>
-      <c r="AN10" s="27"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="11"/>
     </row>
     <row r="11" customHeight="1" spans="1:40">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="12"/>
+      <c r="J11" s="11"/>
       <c r="K11" s="8"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
-      <c r="O11" s="12"/>
+      <c r="O11" s="11"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="12"/>
+      <c r="T11" s="11"/>
       <c r="U11" s="8"/>
       <c r="V11" s="9"/>
       <c r="W11" s="9"/>
       <c r="X11" s="9"/>
-      <c r="Y11" s="12"/>
+      <c r="Y11" s="11"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="9"/>
       <c r="AB11" s="9"/>
       <c r="AC11" s="9"/>
-      <c r="AD11" s="12"/>
+      <c r="AD11" s="11"/>
       <c r="AE11" s="8"/>
       <c r="AF11" s="9"/>
       <c r="AG11" s="9"/>
       <c r="AH11" s="9"/>
-      <c r="AI11" s="12"/>
+      <c r="AI11" s="11"/>
       <c r="AJ11" s="24"/>
       <c r="AK11" s="25"/>
       <c r="AL11" s="25"/>
-      <c r="AM11" s="26"/>
-      <c r="AN11" s="27"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="11"/>
     </row>
     <row r="12" customHeight="1" spans="1:40">
-      <c r="A12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="13"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="13"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="13"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="13"/>
-      <c r="AI12" s="14"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="13"/>
       <c r="AJ12" s="24"/>
       <c r="AK12" s="25"/>
       <c r="AL12" s="25"/>
-      <c r="AM12" s="26"/>
-      <c r="AN12" s="27"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="11"/>
     </row>
     <row r="13" customHeight="1" spans="1:40">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="15"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="17"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="17"/>
-      <c r="AE13" s="15"/>
-      <c r="AF13" s="16"/>
-      <c r="AG13" s="16"/>
-      <c r="AH13" s="16"/>
-      <c r="AI13" s="17"/>
-      <c r="AJ13" s="28"/>
-      <c r="AK13" s="29"/>
-      <c r="AL13" s="29"/>
-      <c r="AM13" s="29"/>
-      <c r="AN13" s="30"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="14"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+      <c r="AI13" s="16"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="27"/>
+      <c r="AL13" s="27"/>
+      <c r="AM13" s="27"/>
+      <c r="AN13" s="28"/>
     </row>
     <row r="14" customHeight="1" spans="1:40">
       <c r="A14" s="5" t="s">
@@ -3125,142 +3356,170 @@
     <row r="15" customHeight="1" spans="1:40">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="11"/>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
-      <c r="I15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="11"/>
       <c r="K15" s="8"/>
       <c r="L15" s="9"/>
-      <c r="N15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="9"/>
       <c r="O15" s="11"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
-      <c r="S15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="9"/>
       <c r="T15" s="11"/>
       <c r="U15" s="8"/>
       <c r="V15" s="9"/>
-      <c r="X15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="9"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="9"/>
-      <c r="AC15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="9"/>
       <c r="AD15" s="11"/>
       <c r="AE15" s="8"/>
       <c r="AF15" s="9"/>
-      <c r="AH15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="9"/>
       <c r="AI15" s="11"/>
       <c r="AJ15" s="24"/>
       <c r="AK15" s="25"/>
       <c r="AL15" s="25"/>
-      <c r="AM15" s="26"/>
-      <c r="AN15" s="27"/>
+      <c r="AM15" s="9"/>
+      <c r="AN15" s="11"/>
     </row>
     <row r="16" customHeight="1" spans="1:40">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="12"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="8"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="12"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="8"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
-      <c r="O16" s="12"/>
+      <c r="O16" s="11"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="12"/>
+      <c r="T16" s="11"/>
       <c r="U16" s="8"/>
       <c r="V16" s="9"/>
       <c r="W16" s="9"/>
       <c r="X16" s="9"/>
-      <c r="Y16" s="12"/>
+      <c r="Y16" s="11"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
-      <c r="AD16" s="12"/>
+      <c r="AD16" s="11"/>
       <c r="AE16" s="8"/>
       <c r="AF16" s="9"/>
       <c r="AG16" s="9"/>
       <c r="AH16" s="9"/>
-      <c r="AI16" s="12"/>
+      <c r="AI16" s="11"/>
       <c r="AJ16" s="24"/>
       <c r="AK16" s="25"/>
       <c r="AL16" s="25"/>
-      <c r="AM16" s="26"/>
-      <c r="AN16" s="27"/>
+      <c r="AM16" s="9"/>
+      <c r="AN16" s="11"/>
     </row>
     <row r="17" customHeight="1" spans="1:40">
-      <c r="A17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="13"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="13"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="13"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="13"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="13"/>
-      <c r="AI17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="13"/>
       <c r="AJ17" s="24"/>
       <c r="AK17" s="25"/>
       <c r="AL17" s="25"/>
-      <c r="AM17" s="26"/>
-      <c r="AN17" s="27"/>
+      <c r="AM17" s="9"/>
+      <c r="AN17" s="11"/>
     </row>
     <row r="18" customHeight="1" spans="1:40">
-      <c r="A18" s="15"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="17"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="17"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="16"/>
-      <c r="AG18" s="16"/>
-      <c r="AH18" s="16"/>
-      <c r="AI18" s="17"/>
-      <c r="AJ18" s="28"/>
-      <c r="AK18" s="29"/>
-      <c r="AL18" s="29"/>
-      <c r="AM18" s="29"/>
-      <c r="AN18" s="30"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="16"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="15"/>
+      <c r="AG18" s="15"/>
+      <c r="AH18" s="15"/>
+      <c r="AI18" s="16"/>
+      <c r="AJ18" s="26"/>
+      <c r="AK18" s="27"/>
+      <c r="AL18" s="27"/>
+      <c r="AM18" s="27"/>
+      <c r="AN18" s="28"/>
     </row>
     <row r="19" customHeight="1" spans="1:40">
       <c r="A19" s="5" t="s">
@@ -3321,142 +3580,170 @@
     <row r="20" customHeight="1" spans="1:40">
       <c r="A20" s="8"/>
       <c r="B20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="11"/>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
-      <c r="I20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="11"/>
       <c r="K20" s="8"/>
       <c r="L20" s="9"/>
-      <c r="N20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="9"/>
       <c r="O20" s="11"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="9"/>
-      <c r="S20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="9"/>
       <c r="T20" s="11"/>
       <c r="U20" s="8"/>
       <c r="V20" s="9"/>
-      <c r="X20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="9"/>
       <c r="Y20" s="11"/>
       <c r="Z20" s="8"/>
       <c r="AA20" s="9"/>
-      <c r="AC20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="9"/>
       <c r="AD20" s="11"/>
       <c r="AE20" s="8"/>
       <c r="AF20" s="9"/>
-      <c r="AH20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="9"/>
       <c r="AI20" s="11"/>
       <c r="AJ20" s="24"/>
       <c r="AK20" s="25"/>
       <c r="AL20" s="25"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="27"/>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="11"/>
     </row>
     <row r="21" customHeight="1" spans="1:40">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="8"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="12"/>
+      <c r="J21" s="11"/>
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="11"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="12"/>
+      <c r="T21" s="11"/>
       <c r="U21" s="8"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
       <c r="X21" s="9"/>
-      <c r="Y21" s="12"/>
+      <c r="Y21" s="11"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
-      <c r="AD21" s="12"/>
+      <c r="AD21" s="11"/>
       <c r="AE21" s="8"/>
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="9"/>
-      <c r="AI21" s="12"/>
+      <c r="AI21" s="11"/>
       <c r="AJ21" s="24"/>
       <c r="AK21" s="25"/>
       <c r="AL21" s="25"/>
-      <c r="AM21" s="26"/>
-      <c r="AN21" s="27"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="11"/>
     </row>
     <row r="22" customHeight="1" spans="1:40">
-      <c r="A22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="13"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="13"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="13"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="13"/>
-      <c r="AD22" s="14"/>
-      <c r="AE22" s="13"/>
-      <c r="AI22" s="14"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="12"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="13"/>
       <c r="AJ22" s="24"/>
       <c r="AK22" s="25"/>
       <c r="AL22" s="25"/>
-      <c r="AM22" s="26"/>
-      <c r="AN22" s="27"/>
+      <c r="AM22" s="9"/>
+      <c r="AN22" s="11"/>
     </row>
     <row r="23" customHeight="1" spans="1:40">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="15"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="17"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="16"/>
-      <c r="AB23" s="16"/>
-      <c r="AC23" s="16"/>
-      <c r="AD23" s="17"/>
-      <c r="AE23" s="15"/>
-      <c r="AF23" s="16"/>
-      <c r="AG23" s="16"/>
-      <c r="AH23" s="16"/>
-      <c r="AI23" s="17"/>
-      <c r="AJ23" s="28"/>
-      <c r="AK23" s="29"/>
-      <c r="AL23" s="29"/>
-      <c r="AM23" s="29"/>
-      <c r="AN23" s="30"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="15"/>
+      <c r="AH23" s="15"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="26"/>
+      <c r="AK23" s="27"/>
+      <c r="AL23" s="27"/>
+      <c r="AM23" s="27"/>
+      <c r="AN23" s="28"/>
     </row>
     <row r="24" customHeight="1" spans="1:40">
       <c r="A24" s="5" t="s">
@@ -3517,142 +3804,170 @@
     <row r="25" customHeight="1" spans="1:40">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="9"/>
       <c r="E25" s="11"/>
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
-      <c r="I25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="11"/>
       <c r="K25" s="8"/>
       <c r="L25" s="9"/>
-      <c r="N25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="9"/>
       <c r="O25" s="11"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="9"/>
-      <c r="S25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="9"/>
       <c r="T25" s="11"/>
       <c r="U25" s="8"/>
       <c r="V25" s="9"/>
-      <c r="X25" s="10"/>
+      <c r="W25" s="10"/>
+      <c r="X25" s="9"/>
       <c r="Y25" s="11"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="9"/>
-      <c r="AC25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="9"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="8"/>
       <c r="AF25" s="9"/>
-      <c r="AH25" s="10"/>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="9"/>
       <c r="AI25" s="11"/>
       <c r="AJ25" s="24"/>
       <c r="AK25" s="25"/>
       <c r="AL25" s="25"/>
-      <c r="AM25" s="26"/>
-      <c r="AN25" s="27"/>
+      <c r="AM25" s="9"/>
+      <c r="AN25" s="11"/>
     </row>
     <row r="26" customHeight="1" spans="1:40">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="12"/>
+      <c r="J26" s="11"/>
       <c r="K26" s="8"/>
       <c r="L26" s="9"/>
       <c r="M26" s="9"/>
       <c r="N26" s="9"/>
-      <c r="O26" s="12"/>
+      <c r="O26" s="11"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
-      <c r="T26" s="12"/>
+      <c r="T26" s="11"/>
       <c r="U26" s="8"/>
       <c r="V26" s="9"/>
       <c r="W26" s="9"/>
       <c r="X26" s="9"/>
-      <c r="Y26" s="12"/>
+      <c r="Y26" s="11"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="9"/>
       <c r="AB26" s="9"/>
       <c r="AC26" s="9"/>
-      <c r="AD26" s="12"/>
+      <c r="AD26" s="11"/>
       <c r="AE26" s="8"/>
       <c r="AF26" s="9"/>
       <c r="AG26" s="9"/>
       <c r="AH26" s="9"/>
-      <c r="AI26" s="12"/>
+      <c r="AI26" s="11"/>
       <c r="AJ26" s="24"/>
       <c r="AK26" s="25"/>
       <c r="AL26" s="25"/>
-      <c r="AM26" s="26"/>
-      <c r="AN26" s="27"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="11"/>
     </row>
     <row r="27" customHeight="1" spans="1:40">
-      <c r="A27" s="13"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="13"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="13"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="13"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="13"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="13"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="13"/>
-      <c r="AI27" s="14"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="12"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="12"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="13"/>
       <c r="AJ27" s="24"/>
       <c r="AK27" s="25"/>
       <c r="AL27" s="25"/>
-      <c r="AM27" s="26"/>
-      <c r="AN27" s="27"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="11"/>
     </row>
     <row r="28" customHeight="1" spans="1:40">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="17"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="17"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="16"/>
-      <c r="AC28" s="16"/>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="16"/>
-      <c r="AG28" s="16"/>
-      <c r="AH28" s="16"/>
-      <c r="AI28" s="17"/>
-      <c r="AJ28" s="28"/>
-      <c r="AK28" s="29"/>
-      <c r="AL28" s="29"/>
-      <c r="AM28" s="29"/>
-      <c r="AN28" s="30"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="16"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="15"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="15"/>
+      <c r="AG28" s="15"/>
+      <c r="AH28" s="15"/>
+      <c r="AI28" s="16"/>
+      <c r="AJ28" s="26"/>
+      <c r="AK28" s="27"/>
+      <c r="AL28" s="27"/>
+      <c r="AM28" s="27"/>
+      <c r="AN28" s="28"/>
     </row>
     <row r="29" customHeight="1" spans="1:40">
       <c r="A29" s="5" t="s">
@@ -3713,142 +4028,170 @@
     <row r="30" customHeight="1" spans="1:40">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="11"/>
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
-      <c r="I30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="11"/>
       <c r="K30" s="8"/>
       <c r="L30" s="9"/>
-      <c r="N30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="9"/>
       <c r="O30" s="11"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="9"/>
-      <c r="S30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="9"/>
       <c r="T30" s="11"/>
       <c r="U30" s="8"/>
       <c r="V30" s="9"/>
-      <c r="X30" s="10"/>
+      <c r="W30" s="10"/>
+      <c r="X30" s="9"/>
       <c r="Y30" s="11"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="9"/>
-      <c r="AC30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="9"/>
       <c r="AD30" s="11"/>
       <c r="AE30" s="8"/>
       <c r="AF30" s="9"/>
-      <c r="AH30" s="10"/>
+      <c r="AG30" s="10"/>
+      <c r="AH30" s="9"/>
       <c r="AI30" s="11"/>
       <c r="AJ30" s="24"/>
       <c r="AK30" s="25"/>
       <c r="AL30" s="25"/>
-      <c r="AM30" s="26"/>
-      <c r="AN30" s="27"/>
+      <c r="AM30" s="9"/>
+      <c r="AN30" s="11"/>
     </row>
     <row r="31" customHeight="1" spans="1:40">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="12"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
-      <c r="J31" s="12"/>
+      <c r="J31" s="11"/>
       <c r="K31" s="8"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
-      <c r="O31" s="12"/>
+      <c r="O31" s="11"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="9"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
-      <c r="T31" s="12"/>
+      <c r="T31" s="11"/>
       <c r="U31" s="8"/>
       <c r="V31" s="9"/>
       <c r="W31" s="9"/>
       <c r="X31" s="9"/>
-      <c r="Y31" s="12"/>
+      <c r="Y31" s="11"/>
       <c r="Z31" s="8"/>
       <c r="AA31" s="9"/>
       <c r="AB31" s="9"/>
       <c r="AC31" s="9"/>
-      <c r="AD31" s="12"/>
+      <c r="AD31" s="11"/>
       <c r="AE31" s="8"/>
       <c r="AF31" s="9"/>
       <c r="AG31" s="9"/>
       <c r="AH31" s="9"/>
-      <c r="AI31" s="12"/>
+      <c r="AI31" s="11"/>
       <c r="AJ31" s="24"/>
       <c r="AK31" s="25"/>
       <c r="AL31" s="25"/>
-      <c r="AM31" s="26"/>
-      <c r="AN31" s="27"/>
+      <c r="AM31" s="9"/>
+      <c r="AN31" s="11"/>
     </row>
     <row r="32" customHeight="1" spans="1:40">
-      <c r="A32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="13"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="13"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="13"/>
-      <c r="T32" s="14"/>
-      <c r="U32" s="13"/>
-      <c r="Y32" s="14"/>
-      <c r="Z32" s="13"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="13"/>
-      <c r="AI32" s="14"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="13"/>
       <c r="AJ32" s="24"/>
       <c r="AK32" s="25"/>
       <c r="AL32" s="25"/>
-      <c r="AM32" s="26"/>
-      <c r="AN32" s="27"/>
+      <c r="AM32" s="9"/>
+      <c r="AN32" s="11"/>
     </row>
     <row r="33" customHeight="1" spans="1:40">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="16"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="16"/>
-      <c r="R33" s="16"/>
-      <c r="S33" s="16"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="15"/>
-      <c r="V33" s="16"/>
-      <c r="W33" s="16"/>
-      <c r="X33" s="16"/>
-      <c r="Y33" s="17"/>
-      <c r="Z33" s="15"/>
-      <c r="AA33" s="16"/>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="16"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="15"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="16"/>
-      <c r="AH33" s="16"/>
-      <c r="AI33" s="17"/>
-      <c r="AJ33" s="28"/>
-      <c r="AK33" s="29"/>
-      <c r="AL33" s="29"/>
-      <c r="AM33" s="29"/>
-      <c r="AN33" s="30"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="16"/>
+      <c r="AJ33" s="26"/>
+      <c r="AK33" s="27"/>
+      <c r="AL33" s="27"/>
+      <c r="AM33" s="27"/>
+      <c r="AN33" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="267">
@@ -3895,13 +4238,6 @@
     <mergeCell ref="AM6:AN6"/>
     <mergeCell ref="AJ7:AL7"/>
     <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="U8:Y8"/>
-    <mergeCell ref="Z8:AD8"/>
-    <mergeCell ref="AE8:AI8"/>
     <mergeCell ref="AJ8:AN8"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="F9:J9"/>
@@ -3938,13 +4274,6 @@
     <mergeCell ref="AM11:AN11"/>
     <mergeCell ref="AJ12:AL12"/>
     <mergeCell ref="AM12:AN12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="P13:T13"/>
-    <mergeCell ref="U13:Y13"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="AE13:AI13"/>
     <mergeCell ref="AJ13:AN13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="F14:J14"/>
@@ -3981,13 +4310,6 @@
     <mergeCell ref="AM16:AN16"/>
     <mergeCell ref="AJ17:AL17"/>
     <mergeCell ref="AM17:AN17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="K18:O18"/>
-    <mergeCell ref="P18:T18"/>
-    <mergeCell ref="U18:Y18"/>
-    <mergeCell ref="Z18:AD18"/>
-    <mergeCell ref="AE18:AI18"/>
     <mergeCell ref="AJ18:AN18"/>
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="F19:J19"/>
@@ -4024,13 +4346,6 @@
     <mergeCell ref="AM21:AN21"/>
     <mergeCell ref="AJ22:AL22"/>
     <mergeCell ref="AM22:AN22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="P23:T23"/>
-    <mergeCell ref="U23:Y23"/>
-    <mergeCell ref="Z23:AD23"/>
-    <mergeCell ref="AE23:AI23"/>
     <mergeCell ref="AJ23:AN23"/>
     <mergeCell ref="A24:E24"/>
     <mergeCell ref="F24:J24"/>
@@ -4067,13 +4382,6 @@
     <mergeCell ref="AM26:AN26"/>
     <mergeCell ref="AJ27:AL27"/>
     <mergeCell ref="AM27:AN27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="P28:T28"/>
-    <mergeCell ref="U28:Y28"/>
-    <mergeCell ref="Z28:AD28"/>
-    <mergeCell ref="AE28:AI28"/>
     <mergeCell ref="AJ28:AN28"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="F29:J29"/>
@@ -4110,15 +4418,50 @@
     <mergeCell ref="AM31:AN31"/>
     <mergeCell ref="AJ32:AL32"/>
     <mergeCell ref="AM32:AN32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="K33:O33"/>
-    <mergeCell ref="P33:T33"/>
-    <mergeCell ref="U33:Y33"/>
-    <mergeCell ref="Z33:AD33"/>
-    <mergeCell ref="AE33:AI33"/>
     <mergeCell ref="AJ33:AN33"/>
     <mergeCell ref="S1:V2"/>
+    <mergeCell ref="A7:E8"/>
+    <mergeCell ref="F7:J8"/>
+    <mergeCell ref="K7:O8"/>
+    <mergeCell ref="P7:T8"/>
+    <mergeCell ref="U7:Y8"/>
+    <mergeCell ref="Z7:AD8"/>
+    <mergeCell ref="AE7:AI8"/>
+    <mergeCell ref="A12:E13"/>
+    <mergeCell ref="F12:J13"/>
+    <mergeCell ref="K12:O13"/>
+    <mergeCell ref="P12:T13"/>
+    <mergeCell ref="U12:Y13"/>
+    <mergeCell ref="Z12:AD13"/>
+    <mergeCell ref="AE12:AI13"/>
+    <mergeCell ref="A17:E18"/>
+    <mergeCell ref="F17:J18"/>
+    <mergeCell ref="K17:O18"/>
+    <mergeCell ref="P17:T18"/>
+    <mergeCell ref="U17:Y18"/>
+    <mergeCell ref="Z17:AD18"/>
+    <mergeCell ref="AE17:AI18"/>
+    <mergeCell ref="A22:E23"/>
+    <mergeCell ref="F22:J23"/>
+    <mergeCell ref="K22:O23"/>
+    <mergeCell ref="P22:T23"/>
+    <mergeCell ref="U22:Y23"/>
+    <mergeCell ref="Z22:AD23"/>
+    <mergeCell ref="AE22:AI23"/>
+    <mergeCell ref="A27:E28"/>
+    <mergeCell ref="F27:J28"/>
+    <mergeCell ref="K27:O28"/>
+    <mergeCell ref="P27:T28"/>
+    <mergeCell ref="U27:Y28"/>
+    <mergeCell ref="Z27:AD28"/>
+    <mergeCell ref="AE27:AI28"/>
+    <mergeCell ref="A32:E33"/>
+    <mergeCell ref="F32:J33"/>
+    <mergeCell ref="K32:O33"/>
+    <mergeCell ref="P32:T33"/>
+    <mergeCell ref="U32:Y33"/>
+    <mergeCell ref="Z32:AD33"/>
+    <mergeCell ref="AE32:AI33"/>
   </mergeCells>
   <pageMargins left="0.389583333333333" right="0.389583333333333" top="1" bottom="0.589583333333333" header="0.309722222222222" footer="0.309722222222222"/>
   <pageSetup paperSize="1" orientation="landscape" horizontalDpi="600"/>

</xml_diff>